<commit_message>
update isa run to reflect current folder structure
</commit_message>
<xml_diff>
--- a/runs/run1/isa.run.xlsx
+++ b/runs/run1/isa.run.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\source\repos\Hackathon_SampleRun\runs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Zimmer\source\repos\Hackathon_SampleRun\runs\run1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09920C95-46B9-4AA6-BDF7-D4C60AFF57A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3F2147-805D-4AAC-89E2-B70BCCE1C5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="750" windowWidth="16200" windowHeight="11423" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4268" yWindow="4185" windowWidth="18225" windowHeight="11423" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="4" r:id="rId1"/>
@@ -187,13 +187,13 @@
     <t>./runs/proteomiqon/run.cwl</t>
   </si>
   <si>
-    <t>./runs/proteomiqon/db/Minimal.db</t>
-  </si>
-  <si>
-    <t>./runs/proteomiqon/psmstats/minimal.qpsm</t>
-  </si>
-  <si>
-    <t>./runs/proteomiqon/db/ChlamyQProt.db</t>
+    <t>./runs/run1/run.cwl</t>
+  </si>
+  <si>
+    <t>./runs/run1/db/Minimal.db</t>
+  </si>
+  <si>
+    <t>./runs/run1/psmstats/minimal.qpsm</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1264,7 +1264,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1294,10 +1294,10 @@
         <v>23</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" s="17"/>
     </row>
@@ -1306,10 +1306,10 @@
         <v>22</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" s="17"/>
     </row>
@@ -1318,10 +1318,10 @@
         <v>17</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D4" s="17"/>
     </row>
@@ -1330,10 +1330,10 @@
         <v>18</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" s="17"/>
     </row>
@@ -1342,10 +1342,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="17"/>
     </row>
@@ -1354,10 +1354,10 @@
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" s="17"/>
     </row>
@@ -1366,10 +1366,10 @@
         <v>20</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="17"/>
     </row>
@@ -1378,10 +1378,10 @@
         <v>20</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D9" s="17"/>
     </row>
@@ -1390,7 +1390,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="17" t="str">
         <f>[1]Dictionary!A6</f>
@@ -1403,7 +1403,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="17" t="str">
         <f>[1]Dictionary!A7</f>

</xml_diff>